<commit_message>
Update config file tags
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,21 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hazenandsawyer-my.sharepoint.com/personal/wraseman_hazenandsawyer_com/Documents/Projects - Active/70047-000 WRF 4954 Reuse Data/Data Analysis/2023-06-06 Demo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HMI103\Desktop\DPR Event Monitoring\live\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="13_ncr:1_{BC199A71-1DC8-494C-B656-190185497D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D990737-6108-467D-9887-AE2AD9E316C1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A069DE7A-41CD-46CD-8655-2A5E73D215C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{E2A42F1A-9299-BA4D-8E30-43A6E9429B06}"/>
+    <workbookView xWindow="5670" yWindow="0" windowWidth="21645" windowHeight="21000" activeTab="1" xr2:uid="{E2A42F1A-9299-BA4D-8E30-43A6E9429B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Tags" sheetId="17" r:id="rId1"/>
     <sheet name="Events" sheetId="18" r:id="rId2"/>
-    <sheet name="Tests" sheetId="16" r:id="rId3"/>
-    <sheet name="Outlier Tests" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="Outlier Tests" sheetId="4" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Actions" localSheetId="3">#REF!</definedName>
+    <definedName name="Actions" localSheetId="2">#REF!</definedName>
     <definedName name="Actions">#REF!</definedName>
     <definedName name="Tag">#REF!</definedName>
     <definedName name="TagDescription">#REF!</definedName>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="171">
   <si>
     <t>Tag</t>
   </si>
@@ -57,9 +56,6 @@
     <t>Process</t>
   </si>
   <si>
-    <t>Parameter</t>
-  </si>
-  <si>
     <t>Units</t>
   </si>
   <si>
@@ -93,9 +89,6 @@
     <t>Filtrate</t>
   </si>
   <si>
-    <t>Turbidity</t>
-  </si>
-  <si>
     <t>NTU</t>
   </si>
   <si>
@@ -150,9 +143,6 @@
     <t>Applied Ozone Dose</t>
   </si>
   <si>
-    <t>Ozone Demand Hach</t>
-  </si>
-  <si>
     <t>Ozone to TOC ratio</t>
   </si>
   <si>
@@ -207,15 +197,9 @@
     <t>UV Feed UVT</t>
   </si>
   <si>
-    <t>UVT</t>
-  </si>
-  <si>
     <t>UV Dose</t>
   </si>
   <si>
-    <t>Dose</t>
-  </si>
-  <si>
     <t>mJ/cm2</t>
   </si>
   <si>
@@ -228,9 +212,6 @@
     <t>UV Intensity Sensor</t>
   </si>
   <si>
-    <t>Intensity</t>
-  </si>
-  <si>
     <t>mW/cm2</t>
   </si>
   <si>
@@ -411,30 +392,6 @@
     <t>Stagnant UV Intensity Sensor</t>
   </si>
   <si>
-    <t>MF Process</t>
-  </si>
-  <si>
-    <t>MF Monitoring</t>
-  </si>
-  <si>
-    <t>RO Process</t>
-  </si>
-  <si>
-    <t>RO Monitoring</t>
-  </si>
-  <si>
-    <t>Events</t>
-  </si>
-  <si>
-    <t>Ozone Meter Error</t>
-  </si>
-  <si>
-    <t>Ozone Demand</t>
-  </si>
-  <si>
-    <t>Total Organic Carbon</t>
-  </si>
-  <si>
     <t>Train A Permeate</t>
   </si>
   <si>
@@ -444,9 +401,6 @@
     <t>UV Intensity</t>
   </si>
   <si>
-    <t xml:space="preserve">Total Chlorine </t>
-  </si>
-  <si>
     <t>RO Permeate Total Chlorine</t>
   </si>
   <si>
@@ -474,69 +428,21 @@
     <t>1 = production. BAC filter status indicates ozone status</t>
   </si>
   <si>
-    <t>Conductivity</t>
-  </si>
-  <si>
     <t>Tag (Units)</t>
   </si>
   <si>
     <t>Ozone LRV via Cryptosporidium</t>
   </si>
   <si>
-    <t>LRV via Cryptosporidium</t>
-  </si>
-  <si>
-    <t>LRV via TOC</t>
-  </si>
-  <si>
     <t>RO LRV via TOC</t>
   </si>
   <si>
-    <t>Normalized Ozone Production Rate Difference Between Measure and Setpoint</t>
-  </si>
-  <si>
     <t>Purpose</t>
   </si>
   <si>
     <t>Value</t>
   </si>
   <si>
-    <t>Datetime Start</t>
-  </si>
-  <si>
-    <t>Datetime End</t>
-  </si>
-  <si>
-    <t>12/20/2022 12:00:00</t>
-  </si>
-  <si>
-    <t>12/20/2022 11:00:00</t>
-  </si>
-  <si>
-    <t>3/24/2023 10:00:00</t>
-  </si>
-  <si>
-    <t>3/22/2023 12:00:00</t>
-  </si>
-  <si>
-    <t>12/20/2022 14:00:00</t>
-  </si>
-  <si>
-    <t>12/20/2022 08:00:00</t>
-  </si>
-  <si>
-    <t>12/20/2022 10:21:00</t>
-  </si>
-  <si>
-    <t>12/20/2022 11:43:00</t>
-  </si>
-  <si>
-    <t>3/24/2023 11:30:00</t>
-  </si>
-  <si>
-    <t>3/22/2023 17:30:00</t>
-  </si>
-  <si>
     <t>Event Text</t>
   </si>
   <si>
@@ -573,15 +479,6 @@
     <t>UVAOP</t>
   </si>
   <si>
-    <t>UVAOP Process</t>
-  </si>
-  <si>
-    <t>UVAOP Monitoring</t>
-  </si>
-  <si>
-    <t>UVAOP WQ</t>
-  </si>
-  <si>
     <t>TagIDs</t>
   </si>
   <si>
@@ -609,68 +506,62 @@
     <t>Meter Drift at Ozone Meter</t>
   </si>
   <si>
-    <t>91, 92, 86, 59</t>
-  </si>
-  <si>
-    <t>Ozone Meter Error OSP 4</t>
-  </si>
-  <si>
-    <t>Ozone Meter Error OSP 7</t>
-  </si>
-  <si>
     <t>OSP 4</t>
   </si>
   <si>
+    <t>Hach</t>
+  </si>
+  <si>
+    <t>Ozone Production Error</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>High Ozone Demand</t>
+  </si>
+  <si>
+    <t>Ozone Demand Hach Meter</t>
+  </si>
+  <si>
+    <t>OSP 4 Hach</t>
+  </si>
+  <si>
+    <t>OSP 7 Hach</t>
+  </si>
+  <si>
+    <t>Ozone Normalized Difference (Across Meters) OSP 4</t>
+  </si>
+  <si>
+    <t>Ozone Demand Rosemount</t>
+  </si>
+  <si>
+    <t>Rosemount</t>
+  </si>
+  <si>
+    <t>Ozone Normalized Difference (Inst vs Rolling) OSP 4 Hach</t>
+  </si>
+  <si>
+    <t>Ozone Normalized Difference (Inst vs Rolling) OSP 7 Hach</t>
+  </si>
+  <si>
+    <t>Ozone Normalized Difference (Across Meters) OSP 7</t>
+  </si>
+  <si>
     <t>OSP 7</t>
   </si>
   <si>
-    <t>Ozone Meter Difference OSP 4</t>
-  </si>
-  <si>
-    <t>Ozone Demand Rosemount Meter</t>
-  </si>
-  <si>
-    <t>Rosemount</t>
-  </si>
-  <si>
-    <t>Hach</t>
-  </si>
-  <si>
-    <t>Ozone Production Error</t>
-  </si>
-  <si>
-    <t>decimal</t>
-  </si>
-  <si>
-    <t>Ozone Process</t>
-  </si>
-  <si>
-    <t>Ozone Monitoring</t>
-  </si>
-  <si>
-    <t>Ozone WQ</t>
-  </si>
-  <si>
-    <t>5/23/2023 13:00:00</t>
-  </si>
-  <si>
-    <t>5/23/2023 16:00:00</t>
-  </si>
-  <si>
-    <t>5/24/2023 12:00:00</t>
-  </si>
-  <si>
-    <t>5/24/2023 14:00:00</t>
-  </si>
-  <si>
-    <t>High Ozone Demand</t>
+    <t>67, 68</t>
+  </si>
+  <si>
+    <t>67, 86, 59</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -717,21 +608,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -741,12 +619,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -808,7 +680,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -847,13 +719,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Input" xfId="2" builtinId="20"/>
@@ -1218,26 +1083,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE57817F-EB9C-47A4-804D-4CF06E690E34}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.453125" customWidth="1"/>
-    <col min="6" max="6" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="46.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -1248,578 +1112,526 @@
         <v>3</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>5</v>
+        <v>128</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F2" t="s">
-        <v>198</v>
-      </c>
-      <c r="G2" s="2" t="str">
-        <f>IF(ISBLANK(F2)=TRUE,B2,B2&amp;" ("&amp;F2&amp;")")</f>
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="2" t="str">
+        <f t="shared" ref="F2:F23" si="0">IF(ISBLANK(E2)=TRUE,B2,B2&amp;" ("&amp;E2&amp;")")</f>
         <v>Ozone Production Error (decimal)</v>
       </c>
-      <c r="H2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>193</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
       <c r="E3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="0"/>
+        <v>Ozone Normalized Difference (Across Meters) OSP 4 (decimal)</v>
+      </c>
+      <c r="G3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="G3" t="str">
-        <f t="shared" ref="G3:G22" si="0">IF(ISBLANK(F3)=TRUE,B3,B3&amp;" ("&amp;F3&amp;")")</f>
-        <v>Ozone Meter Difference OSP 4 (mg/L)</v>
-      </c>
-      <c r="H3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>58</v>
-      </c>
-      <c r="B4" t="s">
-        <v>194</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
       <c r="D4" t="s">
-        <v>195</v>
+        <v>155</v>
       </c>
       <c r="E4" t="s">
-        <v>128</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="str">
+        <v>18</v>
+      </c>
+      <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>Ozone Demand Rosemount Meter (mg/L)</v>
-      </c>
-      <c r="H4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+        <v>Ozone Demand Hach Meter (mg/L)</v>
+      </c>
+      <c r="G4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>146</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="str">
+        <v>9</v>
+      </c>
+      <c r="F5" t="str">
         <f t="shared" si="0"/>
         <v>Ozone LRV via Cryptosporidium (LRV)</v>
       </c>
-      <c r="H5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="str">
+      <c r="F6" t="str">
         <f t="shared" si="0"/>
         <v>MF Filtrate Turbidity (NTU)</v>
       </c>
-      <c r="H6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
-        <v>41</v>
-      </c>
       <c r="E7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" t="str">
+        <v>36</v>
+      </c>
+      <c r="F7" t="str">
         <f t="shared" si="0"/>
         <v>RO Combined Permeate TOC (ug/L)</v>
       </c>
-      <c r="H7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="E8" t="s">
-        <v>143</v>
-      </c>
-      <c r="F8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" t="str">
+        <v>45</v>
+      </c>
+      <c r="F8" t="str">
         <f t="shared" si="0"/>
         <v>RO Train A Permeate Conductivity (uS/cm)</v>
       </c>
-      <c r="H8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="E9" t="s">
-        <v>143</v>
-      </c>
-      <c r="F9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" t="str">
+        <v>45</v>
+      </c>
+      <c r="F9" t="str">
         <f t="shared" si="0"/>
         <v>RO Train B Permeate Conductivity (uS/cm)</v>
       </c>
-      <c r="H9" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>129</v>
-      </c>
-      <c r="F10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" t="str">
+        <v>18</v>
+      </c>
+      <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>RO Feed TOC (ug/L)</v>
-      </c>
-      <c r="H10" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+        <v>RO Feed TOC (mg/L)</v>
+      </c>
+      <c r="G10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>147</v>
-      </c>
-      <c r="F11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" t="str">
+        <v>9</v>
+      </c>
+      <c r="F11" t="str">
         <f t="shared" si="0"/>
         <v>RO LRV via TOC (LRV)</v>
       </c>
-      <c r="H11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" t="str">
+        <v>52</v>
+      </c>
+      <c r="F12" t="str">
         <f t="shared" si="0"/>
         <v>UV Dose (mJ/cm2)</v>
       </c>
-      <c r="H12" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" t="str">
+        <v>56</v>
+      </c>
+      <c r="F13" t="str">
         <f t="shared" si="0"/>
         <v>UV Intensity (mW/cm2)</v>
       </c>
-      <c r="H13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
         <v>19</v>
       </c>
-      <c r="E14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" t="str">
+      <c r="F14" t="str">
         <f t="shared" si="0"/>
         <v>UV Feed UVT (%)</v>
       </c>
-      <c r="H14" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="C15" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>133</v>
-      </c>
-      <c r="F15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" t="str">
+        <v>18</v>
+      </c>
+      <c r="F15" t="str">
         <f t="shared" si="0"/>
         <v>RO Permeate Total Chlorine (mg/L)</v>
       </c>
-      <c r="H15" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" t="str">
+        <v>29</v>
+      </c>
+      <c r="F16" t="str">
         <f t="shared" si="0"/>
         <v>BAC Filter 1 Status</v>
       </c>
+      <c r="G16" t="s">
+        <v>7</v>
+      </c>
       <c r="H16" t="s">
-        <v>8</v>
-      </c>
-      <c r="I16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" t="str">
+        <v>30</v>
+      </c>
+      <c r="F17" t="str">
         <f t="shared" si="0"/>
         <v>BAC Filter 2 Status</v>
       </c>
+      <c r="G17" t="s">
+        <v>7</v>
+      </c>
       <c r="H17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" t="str">
+        <v>13</v>
+      </c>
+      <c r="F18" t="str">
         <f t="shared" si="0"/>
         <v>MF Status</v>
       </c>
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
       <c r="H18" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="C19" t="s">
-        <v>135</v>
-      </c>
-      <c r="E19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" t="str">
+        <v>120</v>
+      </c>
+      <c r="F19" t="str">
         <f t="shared" si="0"/>
         <v>Plantwide Status</v>
       </c>
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
       <c r="H19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>91</v>
       </c>
       <c r="B20" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>191</v>
+        <v>160</v>
       </c>
       <c r="E20" t="s">
-        <v>127</v>
-      </c>
-      <c r="F20" t="s">
-        <v>198</v>
-      </c>
-      <c r="G20" t="str">
+        <v>157</v>
+      </c>
+      <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>Ozone Meter Error OSP 4 (decimal)</v>
-      </c>
-      <c r="H20" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>Ozone Normalized Difference (Inst vs Rolling) OSP 4 Hach (decimal)</v>
+      </c>
+      <c r="G20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>92</v>
       </c>
       <c r="B21" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>192</v>
+        <v>161</v>
       </c>
       <c r="E21" t="s">
-        <v>127</v>
-      </c>
-      <c r="F21" t="s">
-        <v>198</v>
-      </c>
-      <c r="G21" t="str">
+        <v>157</v>
+      </c>
+      <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v>Ozone Meter Error OSP 7 (decimal)</v>
-      </c>
-      <c r="H21" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <v>Ozone Normalized Difference (Inst vs Rolling) OSP 7 Hach (decimal)</v>
+      </c>
+      <c r="G21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>163</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>196</v>
+        <v>164</v>
       </c>
       <c r="E22" t="s">
-        <v>128</v>
-      </c>
-      <c r="F22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>Ozone Demand Rosemount (mg/L)</v>
+      </c>
+      <c r="G22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>68</v>
+      </c>
+      <c r="B23" t="s">
+        <v>167</v>
+      </c>
+      <c r="C23" t="s">
         <v>20</v>
       </c>
-      <c r="G22" t="str">
+      <c r="D23" t="s">
+        <v>168</v>
+      </c>
+      <c r="E23" t="s">
+        <v>157</v>
+      </c>
+      <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v>Ozone Demand Hach (mg/L)</v>
-      </c>
-      <c r="H22" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>94</v>
+        <v>Ozone Normalized Difference (Across Meters) OSP 7 (decimal)</v>
+      </c>
+      <c r="G23" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1832,43 +1644,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E545399E-CD42-4A99-B0FE-F8AB91E65093}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>166</v>
+        <v>135</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>167</v>
+        <v>136</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -1877,125 +1689,125 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>173</v>
+        <v>142</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
       <c r="E7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>174</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
       <c r="E8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="C10" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="D10" t="s">
         <v>3</v>
@@ -2004,66 +1816,66 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C11" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="D11" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
       <c r="E11">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C12" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="D12" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
       <c r="E12">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="C13" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="D13" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="E13">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
         <v>3</v>
@@ -2072,52 +1884,52 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>168</v>
-      </c>
-      <c r="E15">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+      <c r="E15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>206</v>
+        <v>158</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16" t="s">
         <v>170</v>
       </c>
-      <c r="E16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2127,147 +1939,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87240C04-0A08-48C2-8BAD-B6EBDBF2FFAF}">
-  <dimension ref="A1:C11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="A1:C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="22.7265625" customWidth="1"/>
-    <col min="2" max="3" width="18.1796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="21" t="s">
-        <v>199</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="s">
-        <v>200</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>205</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -2276,66 +1947,66 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="28.453125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="28.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="L1" t="s">
-        <v>71</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="B2" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D2,#REF!, 0), 2)</f>
@@ -2346,14 +2017,14 @@
         <v>#REF!</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E2" t="e">
         <f>INDEX(#REF!, MATCH($B2,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G2" s="7">
         <v>-2</v>
@@ -2365,21 +2036,21 @@
         <v>2</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M2" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B3" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D3,#REF!, 0), 2)</f>
@@ -2390,14 +2061,14 @@
         <v>#REF!</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E3" t="e">
         <f>INDEX(#REF!, MATCH($B3,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G3" s="7">
         <v>-2</v>
@@ -2409,21 +2080,21 @@
         <v>2</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M3" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B4" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D4,#REF!, 0), 2)</f>
@@ -2434,14 +2105,14 @@
         <v>#REF!</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E4" t="e">
         <f>INDEX(#REF!, MATCH($B4,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G4" s="7">
         <v>-2</v>
@@ -2453,21 +2124,21 @@
         <v>2</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M4" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B5" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D5,#REF!, 0), 2)</f>
@@ -2478,14 +2149,14 @@
         <v>#REF!</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E5" t="e">
         <f>INDEX(#REF!, MATCH($B5,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G5" s="7">
         <v>-2</v>
@@ -2497,21 +2168,21 @@
         <v>2</v>
       </c>
       <c r="J5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M5" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="M5" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="B6" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D6,#REF!, 0), 2)</f>
@@ -2522,14 +2193,14 @@
         <v>#REF!</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E6" t="e">
         <f>INDEX(#REF!, MATCH($B6,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G6" s="7">
         <v>-2</v>
@@ -2541,21 +2212,21 @@
         <v>2</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M6" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="M6" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="B7" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D7,#REF!, 0), 2)</f>
@@ -2566,14 +2237,14 @@
         <v>#REF!</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E7" t="e">
         <f>INDEX(#REF!, MATCH($B7,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G7" s="7">
         <v>-2</v>
@@ -2585,21 +2256,21 @@
         <v>2</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M7" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="M7" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="B8" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D8,#REF!, 0), 2)</f>
@@ -2610,14 +2281,14 @@
         <v>#REF!</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E8" t="e">
         <f>INDEX(#REF!, MATCH($B8,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G8" s="7">
         <v>-2</v>
@@ -2629,21 +2300,21 @@
         <v>2</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M8" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B9" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D9,#REF!, 0), 2)</f>
@@ -2654,14 +2325,14 @@
         <v>#REF!</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E9" t="e">
         <f>INDEX(#REF!, MATCH($B9,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G9" s="7">
         <v>-2</v>
@@ -2673,21 +2344,21 @@
         <v>2</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M9" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B10" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D10,#REF!, 0), 2)</f>
@@ -2698,14 +2369,14 @@
         <v>#REF!</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E10" t="e">
         <f>INDEX(#REF!, MATCH($B10,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G10" s="7">
         <v>-2</v>
@@ -2717,21 +2388,21 @@
         <v>2</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M10" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B11" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D11,#REF!, 0), 2)</f>
@@ -2742,14 +2413,14 @@
         <v>#REF!</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E11" t="e">
         <f>INDEX(#REF!, MATCH($B11,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G11" s="7">
         <v>-2</v>
@@ -2761,21 +2432,21 @@
         <v>2</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M11" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B12" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D12,#REF!, 0), 2)</f>
@@ -2786,14 +2457,14 @@
         <v>#REF!</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E12" t="e">
         <f>INDEX(#REF!, MATCH($B12,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G12" s="7">
         <v>-1</v>
@@ -2805,21 +2476,21 @@
         <v>1440</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M12" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B13" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D13,#REF!, 0), 2)</f>
@@ -2830,14 +2501,14 @@
         <v>#REF!</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E13" t="e">
         <f>INDEX(#REF!, MATCH($B13,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G13" s="7">
         <v>-1</v>
@@ -2849,21 +2520,21 @@
         <v>1440</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M13" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B14" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D14,#REF!, 0), 2)</f>
@@ -2874,14 +2545,14 @@
         <v>#REF!</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E14" t="e">
         <f>INDEX(#REF!, MATCH($B14,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G14" s="7">
         <v>-1</v>
@@ -2893,21 +2564,21 @@
         <v>1440</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M14" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B15" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D15,#REF!, 0), 2)</f>
@@ -2918,14 +2589,14 @@
         <v>#REF!</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E15" t="e">
         <f>INDEX(#REF!, MATCH($B15,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G15" s="7">
         <v>-1</v>
@@ -2937,21 +2608,21 @@
         <v>1440</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M15" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B16" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D16,#REF!, 0), 2)</f>
@@ -2962,14 +2633,14 @@
         <v>#REF!</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E16" t="e">
         <f>INDEX(#REF!, MATCH($B16,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G16" s="7">
         <v>-1</v>
@@ -2981,21 +2652,21 @@
         <v>1440</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M16" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B17" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D17,#REF!, 0), 2)</f>
@@ -3006,14 +2677,14 @@
         <v>#REF!</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E17" t="e">
         <f>INDEX(#REF!, MATCH($B17,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G17" s="7">
         <v>-1</v>
@@ -3025,21 +2696,21 @@
         <v>1440</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M17" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B18" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D18,#REF!, 0), 2)</f>
@@ -3050,14 +2721,14 @@
         <v>#REF!</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E18" t="e">
         <f>INDEX(#REF!, MATCH($B18,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G18" s="7">
         <v>-1</v>
@@ -3069,21 +2740,21 @@
         <v>1440</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M18" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B19" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D19,#REF!, 0), 2)</f>
@@ -3094,14 +2765,14 @@
         <v>#REF!</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E19" t="e">
         <f>INDEX(#REF!, MATCH($B19,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G19" s="7">
         <v>-1</v>
@@ -3113,21 +2784,21 @@
         <v>1440</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M19" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B20" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D20,#REF!, 0), 2)</f>
@@ -3138,14 +2809,14 @@
         <v>#REF!</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E20" t="e">
         <f>INDEX(#REF!, MATCH($B20,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G20" s="7">
         <v>-1</v>
@@ -3157,21 +2828,21 @@
         <v>1440</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M20" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B21" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D21,#REF!, 0), 2)</f>
@@ -3182,14 +2853,14 @@
         <v>#REF!</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E21" t="e">
         <f>INDEX(#REF!, MATCH($B21,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G21" s="7">
         <v>-1</v>
@@ -3201,21 +2872,21 @@
         <v>1440</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M21" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B22" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D22,#REF!, 0), 2)</f>
@@ -3226,14 +2897,14 @@
         <v>#REF!</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E22" t="e">
         <f>INDEX(#REF!, MATCH($B22,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G22" s="7">
         <v>-2</v>
@@ -3245,21 +2916,21 @@
         <v>2</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M22" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B23" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D23,#REF!, 0), 2)</f>
@@ -3270,14 +2941,14 @@
         <v>#REF!</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E23" t="e">
         <f>INDEX(#REF!, MATCH($B23,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G23" s="7">
         <v>-2</v>
@@ -3289,21 +2960,21 @@
         <v>2</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M23" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B24" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D24,#REF!, 0), 2)</f>
@@ -3314,14 +2985,14 @@
         <v>#REF!</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E24" t="e">
         <f>INDEX(#REF!, MATCH($B24,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G24" s="7">
         <v>-2</v>
@@ -3333,21 +3004,21 @@
         <v>2</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M24" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B25" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D25,#REF!, 0), 2)</f>
@@ -3358,14 +3029,14 @@
         <v>#REF!</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E25" t="e">
         <f>INDEX(#REF!, MATCH($B25,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G25" s="7">
         <v>-2</v>
@@ -3377,21 +3048,21 @@
         <v>2</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K25" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M25" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="M25" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="B26" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D26,#REF!, 0), 2)</f>
@@ -3402,14 +3073,14 @@
         <v>#REF!</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E26" t="e">
         <f>INDEX(#REF!, MATCH($B26,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G26" s="7">
         <v>-2</v>
@@ -3421,21 +3092,21 @@
         <v>2</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M26" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B27" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D27,#REF!, 0), 2)</f>
@@ -3446,14 +3117,14 @@
         <v>#REF!</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E27" t="e">
         <f>INDEX(#REF!, MATCH($B27,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G27" s="7">
         <v>-2</v>
@@ -3465,21 +3136,21 @@
         <v>5</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M27" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B28" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D28,#REF!, 0), 2)</f>
@@ -3490,14 +3161,14 @@
         <v>#REF!</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E28" t="e">
         <f>INDEX(#REF!, MATCH($B28,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G28" s="7">
         <v>-2</v>
@@ -3509,21 +3180,21 @@
         <v>2</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M28" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B29" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D29,#REF!, 0), 2)</f>
@@ -3534,14 +3205,14 @@
         <v>#REF!</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E29" t="e">
         <f>INDEX(#REF!, MATCH($B29,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G29" s="7">
         <v>-2</v>
@@ -3553,21 +3224,21 @@
         <v>2</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M29" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B30" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D30,#REF!, 0), 2)</f>
@@ -3578,14 +3249,14 @@
         <v>#REF!</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E30" t="e">
         <f>INDEX(#REF!, MATCH($B30,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G30" s="7">
         <v>-2</v>
@@ -3597,21 +3268,21 @@
         <v>2</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M30" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B31" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D31,#REF!, 0), 2)</f>
@@ -3622,14 +3293,14 @@
         <v>#REF!</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E31" t="e">
         <f>INDEX(#REF!, MATCH($B31,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G31" s="7">
         <v>-2</v>
@@ -3641,21 +3312,21 @@
         <v>2</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M31" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B32" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D32,#REF!, 0), 2)</f>
@@ -3666,14 +3337,14 @@
         <v>#REF!</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E32" t="e">
         <f>INDEX(#REF!, MATCH($B32,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G32" s="7">
         <v>-2</v>
@@ -3685,21 +3356,21 @@
         <v>2</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M32" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B33" s="4" t="e">
         <f>INDEX(#REF!, MATCH($D33,#REF!, 0), 2)</f>
@@ -3710,14 +3381,14 @@
         <v>#REF!</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E33" t="e">
         <f>INDEX(#REF!, MATCH($B33,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G33" s="7">
         <v>-2</v>
@@ -3729,19 +3400,19 @@
         <v>2</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M33" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" t="e">
         <f>INDEX(#REF!, MATCH($D34,#REF!, 0), 2)</f>
         <v>#REF!</v>
@@ -3751,14 +3422,14 @@
         <v>#REF!</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E34" t="e">
         <f>INDEX(#REF!, MATCH($B34,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G34" s="7">
         <v>-2</v>
@@ -3770,19 +3441,19 @@
         <v>5</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M34" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" t="e">
         <f>INDEX(#REF!, MATCH($D35,#REF!, 0), 2)</f>
         <v>#REF!</v>
@@ -3792,14 +3463,14 @@
         <v>#REF!</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E35" t="e">
         <f>INDEX(#REF!, MATCH($B35,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G35" s="7">
         <v>-2</v>
@@ -3811,19 +3482,19 @@
         <v>5</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K35" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M35" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" t="e">
         <f>INDEX(#REF!, MATCH($D36,#REF!, 0), 2)</f>
         <v>#REF!</v>
@@ -3833,14 +3504,14 @@
         <v>#REF!</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E36" t="e">
         <f>INDEX(#REF!, MATCH($B36,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G36" s="7">
         <v>-2</v>
@@ -3852,19 +3523,19 @@
         <v>10</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M36" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" t="e">
         <f>INDEX(#REF!, MATCH($D37,#REF!, 0), 2)</f>
         <v>#REF!</v>
@@ -3874,14 +3545,14 @@
         <v>#REF!</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E37" t="e">
         <f>INDEX(#REF!, MATCH($B37,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G37" s="7">
         <v>-2</v>
@@ -3893,19 +3564,19 @@
         <v>5</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K37" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M37" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" t="e">
         <f>INDEX(#REF!, MATCH($D38,#REF!, 0), 2)</f>
         <v>#REF!</v>
@@ -3915,14 +3586,14 @@
         <v>#REF!</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E38" t="e">
         <f>INDEX(#REF!, MATCH($B38,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G38" s="7">
         <v>-2</v>
@@ -3934,19 +3605,19 @@
         <v>5</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M38" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="18"/>
       <c r="B39" s="12" t="e">
         <f>INDEX(#REF!, MATCH($D39,#REF!, 0), 2)</f>
@@ -3957,14 +3628,14 @@
         <v>#REF!</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E39" s="12" t="e">
         <f>INDEX(#REF!, MATCH($B39,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G39" s="7">
         <v>-2</v>
@@ -3976,19 +3647,19 @@
         <v>5</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M39" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" t="e">
         <f>INDEX(#REF!, MATCH($D40,#REF!, 0), 2)</f>
         <v>#REF!</v>
@@ -3998,14 +3669,14 @@
         <v>#REF!</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E40" t="e">
         <f>INDEX(#REF!, MATCH($B40,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G40" s="7">
         <v>-2</v>
@@ -4017,19 +3688,19 @@
         <v>5</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M40" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" t="e">
         <f>INDEX(#REF!, MATCH($D41,#REF!, 0), 2)</f>
         <v>#REF!</v>
@@ -4039,14 +3710,14 @@
         <v>#REF!</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E41" t="e">
         <f>INDEX(#REF!, MATCH($B41,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G41" s="7">
         <v>-2</v>
@@ -4058,19 +3729,19 @@
         <v>5</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K41" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M41" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" t="e">
         <f>INDEX(#REF!, MATCH($D42,#REF!, 0), 2)</f>
         <v>#REF!</v>
@@ -4080,14 +3751,14 @@
         <v>#REF!</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E42" t="e">
         <f>INDEX(#REF!, MATCH($B42,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G42" s="7">
         <v>-2</v>
@@ -4099,19 +3770,19 @@
         <v>10</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K42" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L42" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M42" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" t="e">
         <f>INDEX(#REF!, MATCH($D43,#REF!, 0), 2)</f>
         <v>#REF!</v>
@@ -4121,14 +3792,14 @@
         <v>#REF!</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E43" t="e">
         <f>INDEX(#REF!, MATCH($B43,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G43" s="7">
         <v>-2</v>
@@ -4140,19 +3811,19 @@
         <v>5</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K43" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M43" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" t="e">
         <f>INDEX(#REF!, MATCH($D44,#REF!, 0), 2)</f>
         <v>#REF!</v>
@@ -4162,14 +3833,14 @@
         <v>#REF!</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E44" t="e">
         <f>INDEX(#REF!, MATCH($B44,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G44" s="7">
         <v>-2</v>
@@ -4181,19 +3852,19 @@
         <v>5</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K44" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M44" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" t="e">
         <f>INDEX(#REF!, MATCH($D45,#REF!, 0), 2)</f>
         <v>#REF!</v>
@@ -4203,14 +3874,14 @@
         <v>#REF!</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E45" t="e">
         <f>INDEX(#REF!, MATCH($B45,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G45" s="7">
         <v>-2</v>
@@ -4222,19 +3893,19 @@
         <v>5</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K45" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M45" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" t="e">
         <f>INDEX(#REF!, MATCH($D46,#REF!, 0), 2)</f>
         <v>#REF!</v>
@@ -4244,14 +3915,14 @@
         <v>#REF!</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E46" t="e">
         <f>INDEX(#REF!, MATCH($B46,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G46" s="7">
         <v>-2</v>
@@ -4263,19 +3934,19 @@
         <v>5</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M46" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" t="e">
         <f>INDEX(#REF!, MATCH($D47,#REF!, 0), 2)</f>
         <v>#REF!</v>
@@ -4285,14 +3956,14 @@
         <v>#REF!</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E47" t="e">
         <f>INDEX(#REF!, MATCH($B47,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G47" s="7">
         <v>-2</v>
@@ -4304,19 +3975,19 @@
         <v>5</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K47" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M47" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" t="e">
         <f>INDEX(#REF!, MATCH($D48,#REF!, 0), 2)</f>
         <v>#REF!</v>
@@ -4326,14 +3997,14 @@
         <v>#REF!</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E48" t="e">
         <f>INDEX(#REF!, MATCH($B48,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G48" s="7">
         <v>-2</v>
@@ -4345,19 +4016,19 @@
         <v>5</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K48" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M48" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" t="e">
         <f>INDEX(#REF!, MATCH($D49,#REF!, 0), 2)</f>
         <v>#REF!</v>
@@ -4367,14 +4038,14 @@
         <v>#REF!</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E49" t="e">
         <f>INDEX(#REF!, MATCH($B49,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G49" s="7">
         <v>-2</v>
@@ -4386,19 +4057,19 @@
         <v>5</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K49" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M49" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" t="e">
         <f>INDEX(#REF!, MATCH($D50,#REF!, 0), 2)</f>
         <v>#REF!</v>
@@ -4408,14 +4079,14 @@
         <v>#REF!</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E50" t="e">
         <f>INDEX(#REF!, MATCH($B50,#REF!, 0), 7)</f>
         <v>#REF!</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G50" s="7">
         <v>-2</v>
@@ -4427,19 +4098,19 @@
         <v>5</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K50" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M50" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51"/>
       <c r="D51"/>
       <c r="G51"/>
@@ -4449,7 +4120,7 @@
       <c r="K51"/>
       <c r="M51"/>
     </row>
-    <row r="52" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52"/>
       <c r="D52"/>
       <c r="G52"/>
@@ -4459,7 +4130,7 @@
       <c r="K52"/>
       <c r="M52"/>
     </row>
-    <row r="53" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53"/>
       <c r="D53"/>
       <c r="G53"/>
@@ -4469,7 +4140,7 @@
       <c r="K53"/>
       <c r="M53"/>
     </row>
-    <row r="54" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54"/>
       <c r="D54"/>
       <c r="G54"/>
@@ -4479,7 +4150,7 @@
       <c r="K54"/>
       <c r="M54"/>
     </row>
-    <row r="55" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55"/>
       <c r="D55"/>
       <c r="G55"/>
@@ -4489,7 +4160,7 @@
       <c r="K55"/>
       <c r="M55"/>
     </row>
-    <row r="56" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56"/>
       <c r="D56"/>
       <c r="G56"/>
@@ -4499,7 +4170,7 @@
       <c r="K56"/>
       <c r="M56"/>
     </row>
-    <row r="57" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57"/>
       <c r="D57"/>
       <c r="G57"/>
@@ -4509,7 +4180,7 @@
       <c r="K57"/>
       <c r="M57"/>
     </row>
-    <row r="58" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58"/>
       <c r="D58"/>
       <c r="G58"/>
@@ -4519,7 +4190,7 @@
       <c r="K58"/>
       <c r="M58"/>
     </row>
-    <row r="59" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59"/>
       <c r="D59"/>
       <c r="G59"/>
@@ -4529,7 +4200,7 @@
       <c r="K59"/>
       <c r="M59"/>
     </row>
-    <row r="60" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60"/>
       <c r="D60"/>
       <c r="G60"/>
@@ -4539,7 +4210,7 @@
       <c r="K60"/>
       <c r="M60"/>
     </row>
-    <row r="61" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61"/>
       <c r="D61"/>
       <c r="G61"/>
@@ -4549,7 +4220,7 @@
       <c r="K61"/>
       <c r="M61"/>
     </row>
-    <row r="62" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62"/>
       <c r="D62"/>
       <c r="G62"/>
@@ -4559,7 +4230,7 @@
       <c r="K62"/>
       <c r="M62"/>
     </row>
-    <row r="63" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63"/>
       <c r="D63"/>
       <c r="G63"/>
@@ -4569,7 +4240,7 @@
       <c r="K63"/>
       <c r="M63"/>
     </row>
-    <row r="64" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64"/>
       <c r="D64"/>
       <c r="G64"/>
@@ -4579,7 +4250,7 @@
       <c r="K64"/>
       <c r="M64"/>
     </row>
-    <row r="65" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65"/>
       <c r="D65"/>
       <c r="G65"/>
@@ -4589,7 +4260,7 @@
       <c r="K65"/>
       <c r="M65"/>
     </row>
-    <row r="66" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66"/>
       <c r="D66"/>
       <c r="G66"/>
@@ -4599,7 +4270,7 @@
       <c r="K66"/>
       <c r="M66"/>
     </row>
-    <row r="67" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67"/>
       <c r="D67"/>
       <c r="G67"/>
@@ -4609,39 +4280,39 @@
       <c r="K67"/>
       <c r="M67"/>
     </row>
-    <row r="68" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="69" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="70" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="71" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="72" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="73" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="74" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="75" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="76" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="77" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="78" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="79" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="80" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="81" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="82" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="83" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="84" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="85" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="86" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="87" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="88" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="89" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="90" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="91" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="92" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="93" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="94" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="95" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="96" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="97" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="98" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="99" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="100" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="68" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
@@ -4660,6 +4331,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="658658ab-61c7-4ace-9541-96393b4e7795">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Job_x0020_No. xmlns="5e8f08ee-c940-4e9f-8f1c-433053dacb57" xsi:nil="true"/>
+    <TaxCatchAll xmlns="5e8f08ee-c940-4e9f-8f1c-433053dacb57" xsi:nil="true"/>
+    <la4a482e7a5c451c849f25095c650518 xmlns="5e8f08ee-c940-4e9f-8f1c-433053dacb57">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </la4a482e7a5c451c849f25095c650518>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004985D65EB6EA464FBB61A0218386233E" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c0ba5510b9f9d58a5c82dbd919b6a69">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5e8f08ee-c940-4e9f-8f1c-433053dacb57" xmlns:ns3="658658ab-61c7-4ace-9541-96393b4e7795" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e2a7fca07ab34d47e34b7959a48212" ns2:_="" ns3:_="">
     <xsd:import namespace="5e8f08ee-c940-4e9f-8f1c-433053dacb57"/>
@@ -4890,36 +4585,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="fa60db12-2b6a-4eb8-baad-584f0c7a05b3" ContentTypeId="0x0101" PreviousValue="false"/>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B3B4C48-A42C-4846-AD45-92BCCCA104B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="658658ab-61c7-4ace-9541-96393b4e7795">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Job_x0020_No. xmlns="5e8f08ee-c940-4e9f-8f1c-433053dacb57" xsi:nil="true"/>
-    <TaxCatchAll xmlns="5e8f08ee-c940-4e9f-8f1c-433053dacb57" xsi:nil="true"/>
-    <la4a482e7a5c451c849f25095c650518 xmlns="5e8f08ee-c940-4e9f-8f1c-433053dacb57">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </la4a482e7a5c451c849f25095c650518>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9B9F844-E1F7-48B4-A346-AEEE18C3E98B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="658658ab-61c7-4ace-9541-96393b4e7795"/>
+    <ds:schemaRef ds:uri="5e8f08ee-c940-4e9f-8f1c-433053dacb57"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A968F4-6407-42DF-BBB5-74DF6FA8F068}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4938,29 +4628,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F855DD2-37BB-4AFD-B2DD-E02F133B9043}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B3B4C48-A42C-4846-AD45-92BCCCA104B5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9B9F844-E1F7-48B4-A346-AEEE18C3E98B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="658658ab-61c7-4ace-9541-96393b4e7795"/>
-    <ds:schemaRef ds:uri="5e8f08ee-c940-4e9f-8f1c-433053dacb57"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update ozone norm diff tag from 67 to 91 where applicable
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HMI103\Desktop\DPR Event Monitoring\live\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\dpr-event-detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A069DE7A-41CD-46CD-8655-2A5E73D215C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104DF193-F362-4379-AD5B-738FFD0FB58A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5670" yWindow="0" windowWidth="21645" windowHeight="21000" activeTab="1" xr2:uid="{E2A42F1A-9299-BA4D-8E30-43A6E9429B06}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E2A42F1A-9299-BA4D-8E30-43A6E9429B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Tags" sheetId="17" r:id="rId1"/>
@@ -554,7 +554,7 @@
     <t>67, 68</t>
   </si>
   <si>
-    <t>67, 86, 59</t>
+    <t>91, 86, 59</t>
   </si>
 </sst>
 </file>
@@ -1645,7 +1645,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4332,29 +4332,10 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="fa60db12-2b6a-4eb8-baad-584f0c7a05b3" ContentTypeId="0x0101" PreviousValue="false"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="658658ab-61c7-4ace-9541-96393b4e7795">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Job_x0020_No. xmlns="5e8f08ee-c940-4e9f-8f1c-433053dacb57" xsi:nil="true"/>
-    <TaxCatchAll xmlns="5e8f08ee-c940-4e9f-8f1c-433053dacb57" xsi:nil="true"/>
-    <la4a482e7a5c451c849f25095c650518 xmlns="5e8f08ee-c940-4e9f-8f1c-433053dacb57">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </la4a482e7a5c451c849f25095c650518>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004985D65EB6EA464FBB61A0218386233E" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c0ba5510b9f9d58a5c82dbd919b6a69">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5e8f08ee-c940-4e9f-8f1c-433053dacb57" xmlns:ns3="658658ab-61c7-4ace-9541-96393b4e7795" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e2a7fca07ab34d47e34b7959a48212" ns2:_="" ns3:_="">
     <xsd:import namespace="5e8f08ee-c940-4e9f-8f1c-433053dacb57"/>
@@ -4585,31 +4566,39 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="658658ab-61c7-4ace-9541-96393b4e7795">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Job_x0020_No. xmlns="5e8f08ee-c940-4e9f-8f1c-433053dacb57" xsi:nil="true"/>
+    <TaxCatchAll xmlns="5e8f08ee-c940-4e9f-8f1c-433053dacb57" xsi:nil="true"/>
+    <la4a482e7a5c451c849f25095c650518 xmlns="5e8f08ee-c940-4e9f-8f1c-433053dacb57">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </la4a482e7a5c451c849f25095c650518>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="fa60db12-2b6a-4eb8-baad-584f0c7a05b3" ContentTypeId="0x0101" PreviousValue="false"/>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B3B4C48-A42C-4846-AD45-92BCCCA104B5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F855DD2-37BB-4AFD-B2DD-E02F133B9043}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9B9F844-E1F7-48B4-A346-AEEE18C3E98B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="658658ab-61c7-4ace-9541-96393b4e7795"/>
-    <ds:schemaRef ds:uri="5e8f08ee-c940-4e9f-8f1c-433053dacb57"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A968F4-6407-42DF-BBB5-74DF6FA8F068}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4628,10 +4617,21 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9B9F844-E1F7-48B4-A346-AEEE18C3E98B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="658658ab-61c7-4ace-9541-96393b4e7795"/>
+    <ds:schemaRef ds:uri="5e8f08ee-c940-4e9f-8f1c-433053dacb57"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F855DD2-37BB-4AFD-B2DD-E02F133B9043}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B3B4C48-A42C-4846-AD45-92BCCCA104B5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>